<commit_message>
Actualizacion y reduccion de consultas, cambio a views exitoso
</commit_message>
<xml_diff>
--- a/Diligencia_No_Afiliados.xlsx
+++ b/Diligencia_No_Afiliados.xlsx
@@ -446,66 +446,66 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>MANU VILLEDA</v>
+        <v>HECTOR ALVARADO</v>
       </c>
       <c r="B2" t="str">
-        <v>1415-1998-01225</v>
+        <v>0401199021421</v>
       </c>
       <c r="C2" t="str">
-        <v>Hermano (a)</v>
+        <v>Ningun parentesco</v>
       </c>
       <c r="D2" t="str">
         <v>Oficina Principal</v>
       </c>
       <c r="E2" t="str">
-        <v>005-001-141597001</v>
+        <v>005-001-000000052</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>117</v>
       </c>
       <c r="G2" t="str">
-        <v>Venta de una propiedad</v>
+        <v>Herencia</v>
       </c>
       <c r="H2" t="str">
-        <v>Falta de tiempo</v>
+        <v>Esta en el trabajo/negocio</v>
       </c>
       <c r="I2" t="str">
         <v>Depósito</v>
       </c>
       <c r="J2">
-        <v>14500</v>
+        <v>25000</v>
       </c>
       <c r="K2" s="1">
-        <v>44702.721979166665</v>
+        <v>44720.596666666665</v>
       </c>
       <c r="L2" t="str">
         <v>MJVG</v>
       </c>
       <c r="M2" t="str">
-        <v>Nada</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>MANU VILLEDA</v>
+        <v xml:space="preserve">JUAN DAVID PEREZ MENDOZA </v>
       </c>
       <c r="B3" t="str">
-        <v>1415-1998-01225</v>
+        <v>0303030303033</v>
       </c>
       <c r="C3" t="str">
-        <v>Hermano (a)</v>
+        <v>Sobrino (a)</v>
       </c>
       <c r="D3" t="str">
         <v>Oficina Principal</v>
       </c>
       <c r="E3" t="str">
-        <v>005-001-14151998</v>
+        <v>005-001-000002819</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>4671</v>
       </c>
       <c r="G3" t="str">
-        <v>Venta de una propiedad</v>
+        <v>Por Compra o Venta de Naranja</v>
       </c>
       <c r="H3" t="str">
         <v>Falta de tiempo</v>
@@ -514,10 +514,10 @@
         <v>Depósito</v>
       </c>
       <c r="J3">
-        <v>14500</v>
+        <v>10000</v>
       </c>
       <c r="K3" s="1">
-        <v>44704.61928240741</v>
+        <v>44720.38976851852</v>
       </c>
       <c r="L3" t="str">
         <v>MJVG</v>
@@ -528,10 +528,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>MANU VILLEDA</v>
+        <v xml:space="preserve">JUAN JOSE PEREZ RAMIREZ </v>
       </c>
       <c r="B4" t="str">
-        <v>1415-1998-01225</v>
+        <v>0000100012345</v>
       </c>
       <c r="C4" t="str">
         <v>Hermano (a)</v>
@@ -540,31 +540,31 @@
         <v>Oficina Principal</v>
       </c>
       <c r="E4" t="str">
-        <v>005-001-002</v>
+        <v>005-001-000002598</v>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>4367</v>
       </c>
       <c r="G4" t="str">
         <v>Venta de una propiedad</v>
       </c>
       <c r="H4" t="str">
-        <v>Falta de tiempo</v>
+        <v>Esta en el trabajo/negocio</v>
       </c>
       <c r="I4" t="str">
-        <v>Depósito</v>
+        <v>Operación de Unired</v>
       </c>
       <c r="J4">
-        <v>14</v>
+        <v>17000</v>
       </c>
       <c r="K4" s="1">
-        <v>44704.373877314814</v>
+        <v>44714.602638888886</v>
       </c>
       <c r="L4" t="str">
         <v>MJVG</v>
       </c>
       <c r="M4" t="str">
-        <v>mamama</v>
+        <v xml:space="preserve">Prueba de ingresos menores con cliente nuevo </v>
       </c>
     </row>
     <row r="5">
@@ -575,45 +575,45 @@
         <v>1415-1998-01225</v>
       </c>
       <c r="C5" t="str">
-        <v>Hermano (a)</v>
+        <v>Sobrino (a)</v>
       </c>
       <c r="D5" t="str">
         <v>Oficina Principal</v>
       </c>
       <c r="E5" t="str">
-        <v>005-001-002</v>
+        <v>005-1-2598</v>
       </c>
       <c r="F5">
-        <v>15</v>
+        <v>4368</v>
       </c>
       <c r="G5" t="str">
-        <v>Venta de una propiedad</v>
+        <v>Préstamo obtenido</v>
       </c>
       <c r="H5" t="str">
-        <v>Falta de tiempo</v>
+        <v>No queria venir</v>
       </c>
       <c r="I5" t="str">
         <v>Depósito</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>100000</v>
       </c>
       <c r="K5" s="1">
-        <v>44708.64915509259</v>
+        <v>44713.413310185184</v>
       </c>
       <c r="L5" t="str">
         <v>MJVG</v>
       </c>
       <c r="M5" t="str">
-        <v>Prueba de fecha</v>
+        <v>prueba</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>MANU VILLEDA</v>
+        <v xml:space="preserve">NICOLL MARTÍNEZ </v>
       </c>
       <c r="B6" t="str">
-        <v>1415-1998-01225</v>
+        <v>0401-2001-01227</v>
       </c>
       <c r="C6" t="str">
         <v>Hermano (a)</v>
@@ -622,7 +622,7 @@
         <v>Oficina Principal</v>
       </c>
       <c r="E6" t="str">
-        <v>005-002-17589</v>
+        <v>005-001-14759</v>
       </c>
       <c r="F6">
         <v>15</v>
@@ -637,16 +637,16 @@
         <v>Depósito</v>
       </c>
       <c r="J6">
-        <v>150000</v>
+        <v>150001</v>
       </c>
       <c r="K6" s="1">
-        <v>44711.45756944444</v>
+        <v>44711.483252314814</v>
       </c>
       <c r="L6" t="str">
         <v>MJVG</v>
       </c>
       <c r="M6" t="str">
-        <v>Hola</v>
+        <v>hola</v>
       </c>
     </row>
     <row r="7">
@@ -698,37 +698,37 @@
         <v>1415-1998-01225</v>
       </c>
       <c r="C8" t="str">
-        <v>Sobrino (a)</v>
+        <v>Hermano (a)</v>
       </c>
       <c r="D8" t="str">
         <v>Oficina Principal</v>
       </c>
       <c r="E8" t="str">
-        <v>005-1-2598</v>
+        <v>005-002-17589</v>
       </c>
       <c r="F8">
-        <v>4368</v>
+        <v>15</v>
       </c>
       <c r="G8" t="str">
-        <v>Préstamo obtenido</v>
+        <v>Venta de una propiedad</v>
       </c>
       <c r="H8" t="str">
-        <v>No queria venir</v>
+        <v>Falta de tiempo</v>
       </c>
       <c r="I8" t="str">
         <v>Depósito</v>
       </c>
       <c r="J8">
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="K8" s="1">
-        <v>44713.413310185184</v>
+        <v>44711.45756944444</v>
       </c>
       <c r="L8" t="str">
         <v>MJVG</v>
       </c>
       <c r="M8" t="str">
-        <v>prueba</v>
+        <v>Hola</v>
       </c>
     </row>
     <row r="9">
@@ -774,10 +774,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v xml:space="preserve">NICOLL MARTÍNEZ </v>
+        <v>MANU VILLEDA</v>
       </c>
       <c r="B10" t="str">
-        <v>0401-2001-01227</v>
+        <v>1415-1998-01225</v>
       </c>
       <c r="C10" t="str">
         <v>Hermano (a)</v>
@@ -786,7 +786,7 @@
         <v>Oficina Principal</v>
       </c>
       <c r="E10" t="str">
-        <v>005-001-14759</v>
+        <v>005-001-002</v>
       </c>
       <c r="F10">
         <v>15</v>
@@ -801,24 +801,24 @@
         <v>Depósito</v>
       </c>
       <c r="J10">
-        <v>150001</v>
+        <v>3</v>
       </c>
       <c r="K10" s="1">
-        <v>44711.483252314814</v>
+        <v>44708.64915509259</v>
       </c>
       <c r="L10" t="str">
         <v>MJVG</v>
       </c>
       <c r="M10" t="str">
-        <v>hola</v>
+        <v>Prueba de fecha</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v xml:space="preserve">JUAN JOSE PEREZ RAMIREZ </v>
+        <v>MANU VILLEDA</v>
       </c>
       <c r="B11" t="str">
-        <v>0000100012345</v>
+        <v>1415-1998-01225</v>
       </c>
       <c r="C11" t="str">
         <v>Hermano (a)</v>
@@ -827,54 +827,54 @@
         <v>Oficina Principal</v>
       </c>
       <c r="E11" t="str">
-        <v>005-001-000002598</v>
+        <v>005-001-14151998</v>
       </c>
       <c r="F11">
-        <v>4367</v>
+        <v>15</v>
       </c>
       <c r="G11" t="str">
         <v>Venta de una propiedad</v>
       </c>
       <c r="H11" t="str">
-        <v>Esta en el trabajo/negocio</v>
+        <v>Falta de tiempo</v>
       </c>
       <c r="I11" t="str">
-        <v>Operación de Unired</v>
+        <v>Depósito</v>
       </c>
       <c r="J11">
-        <v>17000</v>
+        <v>14500</v>
       </c>
       <c r="K11" s="1">
-        <v>44714.602638888886</v>
+        <v>44704.61928240741</v>
       </c>
       <c r="L11" t="str">
         <v>MJVG</v>
       </c>
       <c r="M11" t="str">
-        <v xml:space="preserve">Prueba de ingresos menores con cliente nuevo </v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v xml:space="preserve">JUAN DAVID PEREZ MENDOZA </v>
+        <v>MANU VILLEDA</v>
       </c>
       <c r="B12" t="str">
-        <v>0303030303033</v>
+        <v>1415-1998-01225</v>
       </c>
       <c r="C12" t="str">
-        <v>Sobrino (a)</v>
+        <v>Hermano (a)</v>
       </c>
       <c r="D12" t="str">
         <v>Oficina Principal</v>
       </c>
       <c r="E12" t="str">
-        <v>005-001-000002819</v>
+        <v>005-001-002</v>
       </c>
       <c r="F12">
-        <v>4671</v>
+        <v>15</v>
       </c>
       <c r="G12" t="str">
-        <v>Por Compra o Venta de Naranja</v>
+        <v>Venta de una propiedad</v>
       </c>
       <c r="H12" t="str">
         <v>Falta de tiempo</v>
@@ -883,57 +883,57 @@
         <v>Depósito</v>
       </c>
       <c r="J12">
-        <v>10000</v>
+        <v>14</v>
       </c>
       <c r="K12" s="1">
-        <v>44720.38976851852</v>
+        <v>44704.373877314814</v>
       </c>
       <c r="L12" t="str">
         <v>MJVG</v>
       </c>
       <c r="M12" t="str">
-        <v/>
+        <v>mamama</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>HECTOR ALVARADO</v>
+        <v>MANU VILLEDA</v>
       </c>
       <c r="B13" t="str">
-        <v>0401199021421</v>
+        <v>1415-1998-01225</v>
       </c>
       <c r="C13" t="str">
-        <v>Ningun parentesco</v>
+        <v>Hermano (a)</v>
       </c>
       <c r="D13" t="str">
         <v>Oficina Principal</v>
       </c>
       <c r="E13" t="str">
-        <v>005-001-000000052</v>
+        <v>005-001-141597001</v>
       </c>
       <c r="F13">
-        <v>117</v>
+        <v>15</v>
       </c>
       <c r="G13" t="str">
-        <v>Herencia</v>
+        <v>Venta de una propiedad</v>
       </c>
       <c r="H13" t="str">
-        <v>Esta en el trabajo/negocio</v>
+        <v>Falta de tiempo</v>
       </c>
       <c r="I13" t="str">
         <v>Depósito</v>
       </c>
       <c r="J13">
-        <v>25000</v>
+        <v>14500</v>
       </c>
       <c r="K13" s="1">
-        <v>44720.596666666665</v>
+        <v>44702.721979166665</v>
       </c>
       <c r="L13" t="str">
         <v>MJVG</v>
       </c>
       <c r="M13" t="str">
-        <v/>
+        <v>Nada</v>
       </c>
     </row>
   </sheetData>

</xml_diff>